<commit_message>
solved architecture & analyzed code
</commit_message>
<xml_diff>
--- a/Docs/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01_ReviewReport.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inspectare" sheetId="1" r:id="rId1"/>
+    <sheet name="Arhitectura" sheetId="2" r:id="rId2"/>
+    <sheet name="Cod Sursa" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
   <si>
     <t>Nr.</t>
   </si>
@@ -108,6 +110,138 @@
   </si>
   <si>
     <t>30 min</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>Is the overall organization of the program clear, including good architectural overview?</t>
+  </si>
+  <si>
+    <t>Is the subsystem and package partitioning and layering logically consistent?</t>
+  </si>
+  <si>
+    <t>Does the architecture account for all of the requirements?</t>
+  </si>
+  <si>
+    <t>Are the classes in a subsystem supporting the services identified for the subsystem?</t>
+  </si>
+  <si>
+    <t>Is there a coherent error handling strategy provided?</t>
+  </si>
+  <si>
+    <t>Have classic design patterns been considered where they might be incorporated into the architecture?</t>
+  </si>
+  <si>
+    <t>Is the name and description of each class clearly reflecting the played role ?</t>
+  </si>
+  <si>
+    <t>Is the description of each class accurately capturing the responsibilities of the class?</t>
+  </si>
+  <si>
+    <t>Are the role names of aggregations and associations accurately describing the relationship between the related classes?</t>
+  </si>
+  <si>
+    <t>Are the key entity classes and their relationships consistent with the business model (if it exists), domain model (if it exists), requirements?</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>C02</t>
+  </si>
+  <si>
+    <t>C03</t>
+  </si>
+  <si>
+    <t>C04</t>
+  </si>
+  <si>
+    <t>C05</t>
+  </si>
+  <si>
+    <t>C06</t>
+  </si>
+  <si>
+    <t>C07</t>
+  </si>
+  <si>
+    <t>C08</t>
+  </si>
+  <si>
+    <t>C09</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>Decision logic is erroneous or inadequate</t>
+  </si>
+  <si>
+    <t>Branching is erroneous.</t>
+  </si>
+  <si>
+    <t>There are undefined loop terminations.</t>
+  </si>
+  <si>
+    <t>I/O format errors exist.</t>
+  </si>
+  <si>
+    <t>Subprogram invocations are violated.</t>
+  </si>
+  <si>
+    <t>There are errors in preparing or processing input data.</t>
+  </si>
+  <si>
+    <t>Output processing errors exist.</t>
+  </si>
+  <si>
+    <t>Error message processing errors exist.</t>
+  </si>
+  <si>
+    <t>There is confusion in the use of parameters.</t>
+  </si>
+  <si>
+    <t>There are errors in loop counters</t>
+  </si>
+  <si>
+    <t>Errors are made in writing out variable names</t>
+  </si>
+  <si>
+    <t>Variable type and dimensions are incorrectly declared</t>
   </si>
 </sst>
 </file>
@@ -132,15 +266,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -148,17 +288,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -443,131 +603,132 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" style="1" customWidth="1"/>
     <col min="7" max="7" width="4.42578125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -575,4 +736,307 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="71.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="G3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="49.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>